<commit_message>
average moves per algorithm per grid
</commit_message>
<xml_diff>
--- a/results/average_moves_per_algorithm.xlsx
+++ b/results/average_moves_per_algorithm.xlsx
@@ -24,26 +24,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
-  <si>
-    <t>algorithm</t>
-  </si>
-  <si>
-    <t>#moves</t>
-  </si>
-  <si>
-    <t>#games</t>
-  </si>
-  <si>
-    <t>random</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>algoritme</t>
+  </si>
+  <si>
+    <t>single step, normal win</t>
+  </si>
+  <si>
+    <t>single step, path free win</t>
+  </si>
+  <si>
+    <t>max step, path free win</t>
+  </si>
+  <si>
+    <t>max step, path free win, non recurrent</t>
+  </si>
+  <si>
+    <t>average moves 6x6 game #1</t>
+  </si>
+  <si>
+    <t>amount of measurements</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>1 mln</t>
+  </si>
+  <si>
+    <t>average moves 9x9 game #4</t>
+  </si>
+  <si>
+    <t>1k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -71,8 +100,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -353,70 +388,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" s="2">
+        <v>597.41656999999998</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="2">
+        <v>103.05871999999999</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>210003</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
+      <c r="B4" s="2">
+        <v>101.35699</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>67187</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>42092</v>
-      </c>
-      <c r="D5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>135287</v>
-      </c>
-      <c r="D6">
-        <v>5000</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>90.427689999999998</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6408.165</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added results from new queue algorithm
</commit_message>
<xml_diff>
--- a/results/average_moves_per_algorithm.xlsx
+++ b/results/average_moves_per_algorithm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>algoritme</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>1k</t>
+  </si>
+  <si>
+    <t>queue_hiele</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +475,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>19.520630000000001</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some more 9x9 average values
</commit_message>
<xml_diff>
--- a/results/average_moves_per_algorithm.xlsx
+++ b/results/average_moves_per_algorithm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
   <si>
     <t>average moves 6x6 game #1</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>queue</t>
+  </si>
+  <si>
+    <t>10k</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +123,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -133,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -145,6 +154,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -427,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,8 +618,12 @@
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="4">
+        <v>9918.8912</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -625,8 +641,12 @@
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="5">
+        <v>9918</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -645,13 +665,13 @@
         <v>2</v>
       </c>
       <c r="G15" s="2">
-        <v>6408.165</v>
+        <v>6408</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -668,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -683,6 +703,40 @@
       </c>
       <c r="E18" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2">
+        <v>70278</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2">
+        <v>8849</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorganized the results folder. Added plots of average moves per algorithm
</commit_message>
<xml_diff>
--- a/results/average_moves_per_algorithm.xlsx
+++ b/results/average_moves_per_algorithm.xlsx
@@ -104,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +129,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -142,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,6 +163,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -442,7 +451,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +724,7 @@
       <c r="C20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="6">
         <v>70278</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -732,7 +741,7 @@
       <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="6">
         <v>8849</v>
       </c>
       <c r="H21" s="2" t="s">

</xml_diff>